<commit_message>
cleaning 2013 presidential per province ontop of shapes
</commit_message>
<xml_diff>
--- a/data/old_results/2013_presidential/2013Mash_Central_Presidential_Results_Formatted_13-08-2013.xlsx
+++ b/data/old_results/2013_presidential/2013Mash_Central_Presidential_Results_Formatted_13-08-2013.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\office\Desktop\DI\Zimbabwe_election\data\old_results\2013_presidential\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{383BF01E-EB3B-4550-9AA0-1D42AAB0F1B2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9C9A7B45-F551-4DE4-B5EA-D44754078538}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,13 +21,13 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4154" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4162" uniqueCount="914">
   <si>
     <t>Local Authority</t>
   </si>
@@ -2766,6 +2766,9 @@
   </si>
   <si>
     <t>done in shape 3</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -16987,7 +16990,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69D30086-222F-4D8E-B520-7D46EDEDA442}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69D30086-222F-4D8E-B520-7D46EDEDA442}" name="PivotTable6" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -17424,10 +17427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9636D1CF-3F0B-4547-A0C9-041434D3CBBD}">
-  <dimension ref="A3:D15"/>
+  <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17438,7 +17441,12 @@
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="11" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>906</v>
       </c>
@@ -17448,8 +17456,11 @@
       <c r="D3" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -17462,8 +17473,11 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -17473,8 +17487,11 @@
       <c r="D5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>255</v>
       </c>
@@ -17484,8 +17501,11 @@
       <c r="D6" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>188</v>
       </c>
@@ -17495,8 +17515,11 @@
       <c r="D7" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>457</v>
       </c>
@@ -17506,8 +17529,11 @@
       <c r="D8" s="10" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>635</v>
       </c>
@@ -17517,8 +17543,11 @@
       <c r="D9" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>488</v>
       </c>
@@ -17528,8 +17557,11 @@
       <c r="D10" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>812</v>
       </c>
@@ -17539,20 +17571,13 @@
       <c r="D11" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>907</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="11" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>